<commit_message>
Added title to graphs on Data.xlsx
</commit_message>
<xml_diff>
--- a/Lab 5/Data collection/Data.xlsx
+++ b/Lab 5/Data collection/Data.xlsx
@@ -20,7 +20,7 @@
     <sheet name="p12d70" sheetId="9" r:id="rId11"/>
     <sheet name="p12d180" sheetId="10" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -575,6 +575,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=0.1 Kd=0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1369,11 +1388,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132569344"/>
-        <c:axId val="95100928"/>
+        <c:axId val="94868608"/>
+        <c:axId val="94870144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="132569344"/>
+        <c:axId val="94868608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1383,7 +1402,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95100928"/>
+        <c:crossAx val="94870144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1391,7 +1410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95100928"/>
+        <c:axId val="94870144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1402,7 +1421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132569344"/>
+        <c:crossAx val="94868608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1438,6 +1457,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=4.5 Kd=80</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2436,11 +2474,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="228232576"/>
-        <c:axId val="102873344"/>
+        <c:axId val="328784128"/>
+        <c:axId val="328785920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="228232576"/>
+        <c:axId val="328784128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2450,7 +2488,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102873344"/>
+        <c:crossAx val="328785920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2458,7 +2496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102873344"/>
+        <c:axId val="328785920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2469,7 +2507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228232576"/>
+        <c:crossAx val="328784128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2505,6 +2543,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=12 Kd=70</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -3359,11 +3416,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103133568"/>
-        <c:axId val="103135104"/>
+        <c:axId val="363156224"/>
+        <c:axId val="363157760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103133568"/>
+        <c:axId val="363156224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3373,7 +3430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103135104"/>
+        <c:crossAx val="363157760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3381,7 +3438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103135104"/>
+        <c:axId val="363157760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3392,7 +3449,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103133568"/>
+        <c:crossAx val="363156224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3428,6 +3485,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=12 Kd=180</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -4294,11 +4370,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103237120"/>
-        <c:axId val="103238656"/>
+        <c:axId val="402000896"/>
+        <c:axId val="402031360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103237120"/>
+        <c:axId val="402000896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4308,7 +4384,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103238656"/>
+        <c:crossAx val="402031360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4316,7 +4392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103238656"/>
+        <c:axId val="402031360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4327,7 +4403,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103237120"/>
+        <c:crossAx val="402000896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4363,6 +4439,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=5 Kd=0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -5241,11 +5336,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95130752"/>
-        <c:axId val="95132288"/>
+        <c:axId val="95006080"/>
+        <c:axId val="95007872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95130752"/>
+        <c:axId val="95006080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5255,7 +5350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95132288"/>
+        <c:crossAx val="95007872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5263,7 +5358,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95132288"/>
+        <c:axId val="95007872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5274,7 +5369,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95130752"/>
+        <c:crossAx val="95006080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5310,6 +5405,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=0.1 Kd=10</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -6260,11 +6374,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103059840"/>
-        <c:axId val="103061376"/>
+        <c:axId val="104556416"/>
+        <c:axId val="104557952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103059840"/>
+        <c:axId val="104556416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6274,7 +6388,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103061376"/>
+        <c:crossAx val="104557952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6282,7 +6396,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103061376"/>
+        <c:axId val="104557952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6293,7 +6407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103059840"/>
+        <c:crossAx val="104556416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6329,6 +6443,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=0.5 Kd=70</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -7087,11 +7220,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="211035264"/>
-        <c:axId val="211036800"/>
+        <c:axId val="107041152"/>
+        <c:axId val="107042688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="211035264"/>
+        <c:axId val="107041152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7101,7 +7234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211036800"/>
+        <c:crossAx val="107042688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7109,7 +7242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211036800"/>
+        <c:axId val="107042688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7120,7 +7253,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211035264"/>
+        <c:crossAx val="107041152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7156,6 +7289,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=3 Kd=60</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -7926,11 +8078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97152384"/>
-        <c:axId val="97162368"/>
+        <c:axId val="159000832"/>
+        <c:axId val="159002624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97152384"/>
+        <c:axId val="159000832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7940,7 +8092,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97162368"/>
+        <c:crossAx val="159002624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7948,7 +8100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97162368"/>
+        <c:axId val="159002624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7959,7 +8111,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97152384"/>
+        <c:crossAx val="159000832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7995,6 +8147,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=3 Kd=70</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -9017,11 +9188,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="78609408"/>
-        <c:axId val="210277120"/>
+        <c:axId val="197604096"/>
+        <c:axId val="197605632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78609408"/>
+        <c:axId val="197604096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9031,7 +9202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210277120"/>
+        <c:crossAx val="197605632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9039,7 +9210,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210277120"/>
+        <c:axId val="197605632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9050,7 +9221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78609408"/>
+        <c:crossAx val="197604096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9086,6 +9257,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=3 Kd=180</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -10900,11 +11090,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="228796288"/>
-        <c:axId val="228797824"/>
+        <c:axId val="228113408"/>
+        <c:axId val="228115200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="228796288"/>
+        <c:axId val="228113408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10914,7 +11104,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228797824"/>
+        <c:crossAx val="228115200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10922,7 +11112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228797824"/>
+        <c:axId val="228115200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10933,7 +11123,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228796288"/>
+        <c:crossAx val="228113408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10969,6 +11159,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=3.5 Kd=80</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -11823,11 +12032,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98049024"/>
-        <c:axId val="229266176"/>
+        <c:axId val="276162048"/>
+        <c:axId val="276163584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98049024"/>
+        <c:axId val="276162048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11837,7 +12046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="229266176"/>
+        <c:crossAx val="276163584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11845,7 +12054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="229266176"/>
+        <c:axId val="276163584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11856,7 +12065,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98049024"/>
+        <c:crossAx val="276162048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11892,6 +12101,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Kp=4 Kd=70</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -12734,11 +12962,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97404800"/>
-        <c:axId val="97406336"/>
+        <c:axId val="298303488"/>
+        <c:axId val="298305024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97404800"/>
+        <c:axId val="298303488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12748,7 +12976,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97406336"/>
+        <c:crossAx val="298305024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12756,7 +12984,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97406336"/>
+        <c:axId val="298305024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12767,7 +12995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97404800"/>
+        <c:crossAx val="298303488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14594,7 +14822,7 @@
   <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18202,7 +18430,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>(A1+0.4)</f>
+        <f t="shared" ref="A2:A33" si="0">(A1+0.4)</f>
         <v>0.4</v>
       </c>
       <c r="B2">
@@ -18220,7 +18448,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>(A2+0.4)</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="B3">
@@ -18238,7 +18466,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>(A3+0.4)</f>
+        <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="B4">
@@ -18256,7 +18484,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>(A4+0.4)</f>
+        <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
       <c r="B5">
@@ -18274,7 +18502,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>(A5+0.4)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B6">
@@ -18292,7 +18520,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>(A6+0.4)</f>
+        <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
       <c r="B7">
@@ -18310,7 +18538,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>(A7+0.4)</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="B8">
@@ -18328,7 +18556,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>(A8+0.4)</f>
+        <f t="shared" si="0"/>
         <v>3.1999999999999997</v>
       </c>
       <c r="B9">
@@ -18346,7 +18574,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>(A9+0.4)</f>
+        <f t="shared" si="0"/>
         <v>3.5999999999999996</v>
       </c>
       <c r="B10">
@@ -18364,7 +18592,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>(A10+0.4)</f>
+        <f t="shared" si="0"/>
         <v>3.9999999999999996</v>
       </c>
       <c r="B11">
@@ -18382,7 +18610,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>(A11+0.4)</f>
+        <f t="shared" si="0"/>
         <v>4.3999999999999995</v>
       </c>
       <c r="B12">
@@ -18400,7 +18628,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>(A12+0.4)</f>
+        <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
       <c r="B13">
@@ -18418,7 +18646,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>(A13+0.4)</f>
+        <f t="shared" si="0"/>
         <v>5.2</v>
       </c>
       <c r="B14">
@@ -18436,7 +18664,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>(A14+0.4)</f>
+        <f t="shared" si="0"/>
         <v>5.6000000000000005</v>
       </c>
       <c r="B15">
@@ -18454,7 +18682,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>(A15+0.4)</f>
+        <f t="shared" si="0"/>
         <v>6.0000000000000009</v>
       </c>
       <c r="B16">
@@ -18472,7 +18700,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>(A16+0.4)</f>
+        <f t="shared" si="0"/>
         <v>6.4000000000000012</v>
       </c>
       <c r="B17">
@@ -18490,7 +18718,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>(A17+0.4)</f>
+        <f t="shared" si="0"/>
         <v>6.8000000000000016</v>
       </c>
       <c r="B18">
@@ -18508,7 +18736,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>(A18+0.4)</f>
+        <f t="shared" si="0"/>
         <v>7.200000000000002</v>
       </c>
       <c r="B19">
@@ -18526,7 +18754,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>(A19+0.4)</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000023</v>
       </c>
       <c r="B20">
@@ -18544,7 +18772,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>(A20+0.4)</f>
+        <f t="shared" si="0"/>
         <v>8.0000000000000018</v>
       </c>
       <c r="B21">
@@ -18562,7 +18790,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>(A21+0.4)</f>
+        <f t="shared" si="0"/>
         <v>8.4000000000000021</v>
       </c>
       <c r="B22">
@@ -18580,7 +18808,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>(A22+0.4)</f>
+        <f t="shared" si="0"/>
         <v>8.8000000000000025</v>
       </c>
       <c r="B23">
@@ -18598,7 +18826,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>(A23+0.4)</f>
+        <f t="shared" si="0"/>
         <v>9.2000000000000028</v>
       </c>
       <c r="B24">
@@ -18616,7 +18844,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>(A24+0.4)</f>
+        <f t="shared" si="0"/>
         <v>9.6000000000000032</v>
       </c>
       <c r="B25">
@@ -18634,7 +18862,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>(A25+0.4)</f>
+        <f t="shared" si="0"/>
         <v>10.000000000000004</v>
       </c>
       <c r="B26">
@@ -18652,7 +18880,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>(A26+0.4)</f>
+        <f t="shared" si="0"/>
         <v>10.400000000000004</v>
       </c>
       <c r="B27">
@@ -18670,7 +18898,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>(A27+0.4)</f>
+        <f t="shared" si="0"/>
         <v>10.800000000000004</v>
       </c>
       <c r="B28">
@@ -18688,7 +18916,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>(A28+0.4)</f>
+        <f t="shared" si="0"/>
         <v>11.200000000000005</v>
       </c>
       <c r="B29">
@@ -18706,7 +18934,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>(A29+0.4)</f>
+        <f t="shared" si="0"/>
         <v>11.600000000000005</v>
       </c>
       <c r="B30">
@@ -18724,7 +18952,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>(A30+0.4)</f>
+        <f t="shared" si="0"/>
         <v>12.000000000000005</v>
       </c>
       <c r="B31">
@@ -18742,7 +18970,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>(A31+0.4)</f>
+        <f t="shared" si="0"/>
         <v>12.400000000000006</v>
       </c>
       <c r="B32">
@@ -18760,7 +18988,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>(A32+0.4)</f>
+        <f t="shared" si="0"/>
         <v>12.800000000000006</v>
       </c>
       <c r="B33">
@@ -18778,7 +19006,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>(A33+0.4)</f>
+        <f t="shared" ref="A34:A67" si="1">(A33+0.4)</f>
         <v>13.200000000000006</v>
       </c>
       <c r="B34">
@@ -18796,7 +19024,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>(A34+0.4)</f>
+        <f t="shared" si="1"/>
         <v>13.600000000000007</v>
       </c>
       <c r="B35">
@@ -18814,7 +19042,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>(A35+0.4)</f>
+        <f t="shared" si="1"/>
         <v>14.000000000000007</v>
       </c>
       <c r="B36">
@@ -18832,7 +19060,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>(A36+0.4)</f>
+        <f t="shared" si="1"/>
         <v>14.400000000000007</v>
       </c>
       <c r="B37">
@@ -18850,7 +19078,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>(A37+0.4)</f>
+        <f t="shared" si="1"/>
         <v>14.800000000000008</v>
       </c>
       <c r="B38">
@@ -18868,7 +19096,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>(A38+0.4)</f>
+        <f t="shared" si="1"/>
         <v>15.200000000000008</v>
       </c>
       <c r="B39">
@@ -18886,7 +19114,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>(A39+0.4)</f>
+        <f t="shared" si="1"/>
         <v>15.600000000000009</v>
       </c>
       <c r="B40">
@@ -18904,7 +19132,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>(A40+0.4)</f>
+        <f t="shared" si="1"/>
         <v>16.000000000000007</v>
       </c>
       <c r="B41">
@@ -18922,7 +19150,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>(A41+0.4)</f>
+        <f t="shared" si="1"/>
         <v>16.400000000000006</v>
       </c>
       <c r="B42">
@@ -18940,7 +19168,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f>(A42+0.4)</f>
+        <f t="shared" si="1"/>
         <v>16.800000000000004</v>
       </c>
       <c r="B43">
@@ -18958,7 +19186,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f>(A43+0.4)</f>
+        <f t="shared" si="1"/>
         <v>17.200000000000003</v>
       </c>
       <c r="B44">
@@ -18976,7 +19204,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f>(A44+0.4)</f>
+        <f t="shared" si="1"/>
         <v>17.600000000000001</v>
       </c>
       <c r="B45">
@@ -18994,7 +19222,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f>(A45+0.4)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B46">
@@ -19012,7 +19240,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f>(A46+0.4)</f>
+        <f t="shared" si="1"/>
         <v>18.399999999999999</v>
       </c>
       <c r="B47">
@@ -19030,7 +19258,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f>(A47+0.4)</f>
+        <f t="shared" si="1"/>
         <v>18.799999999999997</v>
       </c>
       <c r="B48">
@@ -19048,7 +19276,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f>(A48+0.4)</f>
+        <f t="shared" si="1"/>
         <v>19.199999999999996</v>
       </c>
       <c r="B49">
@@ -19066,7 +19294,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f>(A49+0.4)</f>
+        <f t="shared" si="1"/>
         <v>19.599999999999994</v>
       </c>
       <c r="B50">
@@ -19084,7 +19312,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f>(A50+0.4)</f>
+        <f t="shared" si="1"/>
         <v>19.999999999999993</v>
       </c>
       <c r="B51">
@@ -19102,7 +19330,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f>(A51+0.4)</f>
+        <f t="shared" si="1"/>
         <v>20.399999999999991</v>
       </c>
       <c r="B52">
@@ -19120,7 +19348,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f>(A52+0.4)</f>
+        <f t="shared" si="1"/>
         <v>20.79999999999999</v>
       </c>
       <c r="B53">
@@ -19138,7 +19366,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f>(A53+0.4)</f>
+        <f t="shared" si="1"/>
         <v>21.199999999999989</v>
       </c>
       <c r="B54">
@@ -19156,7 +19384,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f>(A54+0.4)</f>
+        <f t="shared" si="1"/>
         <v>21.599999999999987</v>
       </c>
       <c r="B55">
@@ -19174,7 +19402,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f>(A55+0.4)</f>
+        <f t="shared" si="1"/>
         <v>21.999999999999986</v>
       </c>
       <c r="B56">
@@ -19192,7 +19420,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f>(A56+0.4)</f>
+        <f t="shared" si="1"/>
         <v>22.399999999999984</v>
       </c>
       <c r="B57">
@@ -19210,7 +19438,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f>(A57+0.4)</f>
+        <f t="shared" si="1"/>
         <v>22.799999999999983</v>
       </c>
       <c r="B58">
@@ -19228,7 +19456,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f>(A58+0.4)</f>
+        <f t="shared" si="1"/>
         <v>23.199999999999982</v>
       </c>
       <c r="B59">
@@ -19246,7 +19474,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f>(A59+0.4)</f>
+        <f t="shared" si="1"/>
         <v>23.59999999999998</v>
       </c>
       <c r="B60">
@@ -19264,7 +19492,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f>(A60+0.4)</f>
+        <f t="shared" si="1"/>
         <v>23.999999999999979</v>
       </c>
       <c r="B61">
@@ -19282,7 +19510,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f>(A61+0.4)</f>
+        <f t="shared" si="1"/>
         <v>24.399999999999977</v>
       </c>
       <c r="B62">
@@ -19300,7 +19528,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f>(A62+0.4)</f>
+        <f t="shared" si="1"/>
         <v>24.799999999999976</v>
       </c>
       <c r="B63">
@@ -19318,7 +19546,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f>(A63+0.4)</f>
+        <f t="shared" si="1"/>
         <v>25.199999999999974</v>
       </c>
       <c r="B64">
@@ -19336,7 +19564,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f>(A64+0.4)</f>
+        <f t="shared" si="1"/>
         <v>25.599999999999973</v>
       </c>
       <c r="B65">
@@ -19354,7 +19582,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f>(A65+0.4)</f>
+        <f t="shared" si="1"/>
         <v>25.999999999999972</v>
       </c>
       <c r="B66">
@@ -19372,7 +19600,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f>(A66+0.4)</f>
+        <f t="shared" si="1"/>
         <v>26.39999999999997</v>
       </c>
       <c r="B67">
@@ -19423,7 +19651,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>(A1+0.4)</f>
+        <f t="shared" ref="A2:A33" si="0">(A1+0.4)</f>
         <v>0.4</v>
       </c>
       <c r="B2">
@@ -19441,7 +19669,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>(A2+0.4)</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="B3">
@@ -19459,7 +19687,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>(A3+0.4)</f>
+        <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="B4">
@@ -19477,7 +19705,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>(A4+0.4)</f>
+        <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
       <c r="B5">
@@ -19495,7 +19723,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>(A5+0.4)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B6">
@@ -19513,7 +19741,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>(A6+0.4)</f>
+        <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
       <c r="B7">
@@ -19531,7 +19759,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>(A7+0.4)</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="B8">
@@ -19549,7 +19777,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>(A8+0.4)</f>
+        <f t="shared" si="0"/>
         <v>3.1999999999999997</v>
       </c>
       <c r="B9">
@@ -19567,7 +19795,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>(A9+0.4)</f>
+        <f t="shared" si="0"/>
         <v>3.5999999999999996</v>
       </c>
       <c r="B10">
@@ -19585,7 +19813,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>(A10+0.4)</f>
+        <f t="shared" si="0"/>
         <v>3.9999999999999996</v>
       </c>
       <c r="B11">
@@ -19603,7 +19831,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>(A11+0.4)</f>
+        <f t="shared" si="0"/>
         <v>4.3999999999999995</v>
       </c>
       <c r="B12">
@@ -19621,7 +19849,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>(A12+0.4)</f>
+        <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
       <c r="B13">
@@ -19639,7 +19867,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>(A13+0.4)</f>
+        <f t="shared" si="0"/>
         <v>5.2</v>
       </c>
       <c r="B14">
@@ -19657,7 +19885,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>(A14+0.4)</f>
+        <f t="shared" si="0"/>
         <v>5.6000000000000005</v>
       </c>
       <c r="B15">
@@ -19675,7 +19903,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>(A15+0.4)</f>
+        <f t="shared" si="0"/>
         <v>6.0000000000000009</v>
       </c>
       <c r="B16">
@@ -19693,7 +19921,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>(A16+0.4)</f>
+        <f t="shared" si="0"/>
         <v>6.4000000000000012</v>
       </c>
       <c r="B17">
@@ -19711,7 +19939,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>(A17+0.4)</f>
+        <f t="shared" si="0"/>
         <v>6.8000000000000016</v>
       </c>
       <c r="B18">
@@ -19729,7 +19957,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>(A18+0.4)</f>
+        <f t="shared" si="0"/>
         <v>7.200000000000002</v>
       </c>
       <c r="B19">
@@ -19747,7 +19975,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>(A19+0.4)</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000023</v>
       </c>
       <c r="B20">
@@ -19765,7 +19993,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>(A20+0.4)</f>
+        <f t="shared" si="0"/>
         <v>8.0000000000000018</v>
       </c>
       <c r="B21">
@@ -19783,7 +20011,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>(A21+0.4)</f>
+        <f t="shared" si="0"/>
         <v>8.4000000000000021</v>
       </c>
       <c r="B22">
@@ -19801,7 +20029,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>(A22+0.4)</f>
+        <f t="shared" si="0"/>
         <v>8.8000000000000025</v>
       </c>
       <c r="B23">
@@ -19819,7 +20047,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>(A23+0.4)</f>
+        <f t="shared" si="0"/>
         <v>9.2000000000000028</v>
       </c>
       <c r="B24">
@@ -19837,7 +20065,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>(A24+0.4)</f>
+        <f t="shared" si="0"/>
         <v>9.6000000000000032</v>
       </c>
       <c r="B25">
@@ -19855,7 +20083,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>(A25+0.4)</f>
+        <f t="shared" si="0"/>
         <v>10.000000000000004</v>
       </c>
       <c r="B26">
@@ -19873,7 +20101,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>(A26+0.4)</f>
+        <f t="shared" si="0"/>
         <v>10.400000000000004</v>
       </c>
       <c r="B27">
@@ -19891,7 +20119,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>(A27+0.4)</f>
+        <f t="shared" si="0"/>
         <v>10.800000000000004</v>
       </c>
       <c r="B28">
@@ -19909,7 +20137,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>(A28+0.4)</f>
+        <f t="shared" si="0"/>
         <v>11.200000000000005</v>
       </c>
       <c r="B29">
@@ -19927,7 +20155,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>(A29+0.4)</f>
+        <f t="shared" si="0"/>
         <v>11.600000000000005</v>
       </c>
       <c r="B30">
@@ -19945,7 +20173,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>(A30+0.4)</f>
+        <f t="shared" si="0"/>
         <v>12.000000000000005</v>
       </c>
       <c r="B31">
@@ -19963,7 +20191,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>(A31+0.4)</f>
+        <f t="shared" si="0"/>
         <v>12.400000000000006</v>
       </c>
       <c r="B32">
@@ -19981,7 +20209,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>(A32+0.4)</f>
+        <f t="shared" si="0"/>
         <v>12.800000000000006</v>
       </c>
       <c r="B33">
@@ -19999,7 +20227,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>(A33+0.4)</f>
+        <f t="shared" ref="A34:A65" si="1">(A33+0.4)</f>
         <v>13.200000000000006</v>
       </c>
       <c r="B34">
@@ -20017,7 +20245,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>(A34+0.4)</f>
+        <f t="shared" si="1"/>
         <v>13.600000000000007</v>
       </c>
       <c r="B35">
@@ -20035,7 +20263,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>(A35+0.4)</f>
+        <f t="shared" si="1"/>
         <v>14.000000000000007</v>
       </c>
       <c r="B36">
@@ -20053,7 +20281,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>(A36+0.4)</f>
+        <f t="shared" si="1"/>
         <v>14.400000000000007</v>
       </c>
       <c r="B37">
@@ -20071,7 +20299,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>(A37+0.4)</f>
+        <f t="shared" si="1"/>
         <v>14.800000000000008</v>
       </c>
       <c r="B38">
@@ -20089,7 +20317,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>(A38+0.4)</f>
+        <f t="shared" si="1"/>
         <v>15.200000000000008</v>
       </c>
       <c r="B39">
@@ -20107,7 +20335,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>(A39+0.4)</f>
+        <f t="shared" si="1"/>
         <v>15.600000000000009</v>
       </c>
       <c r="B40">
@@ -20125,7 +20353,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>(A40+0.4)</f>
+        <f t="shared" si="1"/>
         <v>16.000000000000007</v>
       </c>
       <c r="B41">
@@ -20143,7 +20371,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>(A41+0.4)</f>
+        <f t="shared" si="1"/>
         <v>16.400000000000006</v>
       </c>
       <c r="B42">
@@ -20161,7 +20389,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f>(A42+0.4)</f>
+        <f t="shared" si="1"/>
         <v>16.800000000000004</v>
       </c>
       <c r="B43">
@@ -20179,7 +20407,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f>(A43+0.4)</f>
+        <f t="shared" si="1"/>
         <v>17.200000000000003</v>
       </c>
       <c r="B44">
@@ -20197,7 +20425,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f>(A44+0.4)</f>
+        <f t="shared" si="1"/>
         <v>17.600000000000001</v>
       </c>
       <c r="B45">
@@ -20215,7 +20443,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f>(A45+0.4)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B46">
@@ -20233,7 +20461,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f>(A46+0.4)</f>
+        <f t="shared" si="1"/>
         <v>18.399999999999999</v>
       </c>
       <c r="B47">
@@ -20251,7 +20479,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f>(A47+0.4)</f>
+        <f t="shared" si="1"/>
         <v>18.799999999999997</v>
       </c>
       <c r="B48">
@@ -20269,7 +20497,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f>(A48+0.4)</f>
+        <f t="shared" si="1"/>
         <v>19.199999999999996</v>
       </c>
       <c r="B49">
@@ -20287,7 +20515,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f>(A49+0.4)</f>
+        <f t="shared" si="1"/>
         <v>19.599999999999994</v>
       </c>
       <c r="B50">
@@ -20305,7 +20533,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f>(A50+0.4)</f>
+        <f t="shared" si="1"/>
         <v>19.999999999999993</v>
       </c>
       <c r="B51">
@@ -20323,7 +20551,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f>(A51+0.4)</f>
+        <f t="shared" si="1"/>
         <v>20.399999999999991</v>
       </c>
       <c r="B52">
@@ -20341,7 +20569,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f>(A52+0.4)</f>
+        <f t="shared" si="1"/>
         <v>20.79999999999999</v>
       </c>
       <c r="B53">
@@ -20359,7 +20587,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f>(A53+0.4)</f>
+        <f t="shared" si="1"/>
         <v>21.199999999999989</v>
       </c>
       <c r="B54">
@@ -20377,7 +20605,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f>(A54+0.4)</f>
+        <f t="shared" si="1"/>
         <v>21.599999999999987</v>
       </c>
       <c r="B55">
@@ -20395,7 +20623,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f>(A55+0.4)</f>
+        <f t="shared" si="1"/>
         <v>21.999999999999986</v>
       </c>
       <c r="B56">
@@ -20413,7 +20641,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f>(A56+0.4)</f>
+        <f t="shared" si="1"/>
         <v>22.399999999999984</v>
       </c>
       <c r="B57">
@@ -20431,7 +20659,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f>(A57+0.4)</f>
+        <f t="shared" si="1"/>
         <v>22.799999999999983</v>
       </c>
       <c r="B58">
@@ -20449,7 +20677,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f>(A58+0.4)</f>
+        <f t="shared" si="1"/>
         <v>23.199999999999982</v>
       </c>
       <c r="B59">
@@ -20467,7 +20695,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f>(A59+0.4)</f>
+        <f t="shared" si="1"/>
         <v>23.59999999999998</v>
       </c>
       <c r="B60">
@@ -20485,7 +20713,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f>(A60+0.4)</f>
+        <f t="shared" si="1"/>
         <v>23.999999999999979</v>
       </c>
       <c r="B61">
@@ -20503,7 +20731,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f>(A61+0.4)</f>
+        <f t="shared" si="1"/>
         <v>24.399999999999977</v>
       </c>
       <c r="B62">
@@ -20521,7 +20749,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f>(A62+0.4)</f>
+        <f t="shared" si="1"/>
         <v>24.799999999999976</v>
       </c>
       <c r="B63">
@@ -20539,7 +20767,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f>(A63+0.4)</f>
+        <f t="shared" si="1"/>
         <v>25.199999999999974</v>
       </c>
       <c r="B64">
@@ -20557,7 +20785,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f>(A64+0.4)</f>
+        <f t="shared" si="1"/>
         <v>25.599999999999973</v>
       </c>
       <c r="B65">
@@ -20575,7 +20803,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f>(A65+0.4)</f>
+        <f t="shared" ref="A66:A73" si="2">(A65+0.4)</f>
         <v>25.999999999999972</v>
       </c>
       <c r="B66">
@@ -20593,7 +20821,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f>(A66+0.4)</f>
+        <f t="shared" si="2"/>
         <v>26.39999999999997</v>
       </c>
       <c r="B67">
@@ -20611,7 +20839,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f>(A67+0.4)</f>
+        <f t="shared" si="2"/>
         <v>26.799999999999969</v>
       </c>
       <c r="B68">
@@ -20629,7 +20857,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f>(A68+0.4)</f>
+        <f t="shared" si="2"/>
         <v>27.199999999999967</v>
       </c>
       <c r="B69">
@@ -20647,7 +20875,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f>(A69+0.4)</f>
+        <f t="shared" si="2"/>
         <v>27.599999999999966</v>
       </c>
       <c r="B70">
@@ -20665,7 +20893,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f>(A70+0.4)</f>
+        <f t="shared" si="2"/>
         <v>27.999999999999964</v>
       </c>
       <c r="B71">
@@ -20683,7 +20911,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f>(A71+0.4)</f>
+        <f t="shared" si="2"/>
         <v>28.399999999999963</v>
       </c>
       <c r="B72">
@@ -20701,7 +20929,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f>(A72+0.4)</f>
+        <f t="shared" si="2"/>
         <v>28.799999999999962</v>
       </c>
       <c r="B73">

</xml_diff>